<commit_message>
With additional work to get Ensemble model up and running
</commit_message>
<xml_diff>
--- a/progress-tracker-table.xlsx
+++ b/progress-tracker-table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelmaclennan/Documents/Learning &amp; Education/2025-04 AI &amp; ML/jigsaw-competition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1555E8-25AB-C84D-8DC9-EE67264FCE39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F471EB-E196-EB4B-9214-901D9A789DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6000" yWindow="5080" windowWidth="28040" windowHeight="17440" xr2:uid="{9D2F94EE-788C-9542-A49A-1C742A203CD2}"/>
   </bookViews>
@@ -16,6 +16,19 @@
     <sheet name="progress-tracker-table" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -981,7 +994,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="186" zoomScaleNormal="186" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>